<commit_message>
Actualizacion pilas Sprint semana 3 y 4
</commit_message>
<xml_diff>
--- a/SPRINT 1/2-Seguimiento/Entregas Sprint-1 plataforma UTP/Entrega 10 Acta de Reunion Semanal de SCRUM No.4/Pila del Sprint 1 v2.xlsx
+++ b/SPRINT 1/2-Seguimiento/Entregas Sprint-1 plataforma UTP/Entrega 10 Acta de Reunion Semanal de SCRUM No.4/Pila del Sprint 1 v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Juan Pablo\Documents\LABORATORIO DE SOFTWARE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARCH\Documents\SourceTree\LaboratorioSW\SPRINT 1\2-Seguimiento\Entregas Sprint-1 plataforma UTP\Entrega 10 Acta de Reunion Semanal de SCRUM No.4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -639,106 +639,109 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1022,7 +1025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -1044,1654 +1047,1654 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
     </row>
     <row r="4" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="D5" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="3" t="s">
+      <c r="F5" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="8" t="s">
+      <c r="M5" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="9"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="33"/>
     </row>
     <row r="6" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="16" t="s">
+      <c r="B6" s="20"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N6" s="17" t="s">
+      <c r="N6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O6" s="17" t="s">
+      <c r="O6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P6" s="18" t="s">
+      <c r="P6" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:16" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="19"/>
-      <c r="C7" s="20" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="I7" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="J7" s="22" t="s">
+      <c r="J7" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="K7" s="20">
-        <v>2</v>
-      </c>
-      <c r="L7" s="23">
+      <c r="K7" s="6">
+        <v>2</v>
+      </c>
+      <c r="L7" s="9">
         <f>K7-(SUM(M7:P7))</f>
         <v>2</v>
       </c>
-      <c r="M7" s="24"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="20"/>
-      <c r="P7" s="25"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="11"/>
     </row>
     <row r="8" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="19"/>
-      <c r="C8" s="20" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="H8" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="J8" s="22" t="s">
+      <c r="J8" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="K8" s="20">
-        <v>2</v>
-      </c>
-      <c r="L8" s="23">
+      <c r="K8" s="6">
+        <v>2</v>
+      </c>
+      <c r="L8" s="9">
         <f t="shared" ref="L8:L45" si="0">K8-(SUM(M8:P8))</f>
         <v>2</v>
       </c>
-      <c r="M8" s="24"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="20"/>
-      <c r="P8" s="25"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="11"/>
     </row>
     <row r="9" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="19"/>
-      <c r="C9" s="20" t="s">
+      <c r="B9" s="5"/>
+      <c r="C9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="F9" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="G9" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="H9" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="I9" s="21" t="s">
+      <c r="I9" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="J9" s="22" t="s">
+      <c r="J9" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="K9" s="20">
+      <c r="K9" s="6">
         <v>8</v>
       </c>
-      <c r="L9" s="23">
+      <c r="L9" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M9" s="24">
-        <v>2</v>
-      </c>
-      <c r="N9" s="20"/>
-      <c r="O9" s="20"/>
-      <c r="P9" s="25"/>
+      <c r="M9" s="10">
+        <v>2</v>
+      </c>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="11"/>
     </row>
     <row r="10" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="19"/>
-      <c r="C10" s="20" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="F10" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="G10" s="20" t="s">
+      <c r="G10" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="H10" s="20" t="s">
+      <c r="H10" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="I10" s="21" t="s">
+      <c r="I10" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="J10" s="22" t="s">
+      <c r="J10" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="K10" s="20">
+      <c r="K10" s="6">
         <v>8</v>
       </c>
-      <c r="L10" s="23">
+      <c r="L10" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M10" s="24">
-        <v>2</v>
-      </c>
-      <c r="N10" s="20"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="25"/>
+      <c r="M10" s="10">
+        <v>2</v>
+      </c>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="11"/>
     </row>
     <row r="11" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="19"/>
-      <c r="C11" s="20" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="F11" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="G11" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="H11" s="20" t="s">
+      <c r="H11" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="I11" s="21" t="s">
+      <c r="I11" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="J11" s="22" t="s">
+      <c r="J11" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="K11" s="20">
+      <c r="K11" s="6">
         <v>8</v>
       </c>
-      <c r="L11" s="23">
+      <c r="L11" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M11" s="24">
-        <v>2</v>
-      </c>
-      <c r="N11" s="20"/>
-      <c r="O11" s="20"/>
-      <c r="P11" s="25"/>
+      <c r="M11" s="10">
+        <v>2</v>
+      </c>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="11"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="19"/>
-      <c r="C12" s="20" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="20" t="s">
+      <c r="F12" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G12" s="20" t="s">
+      <c r="G12" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="H12" s="20" t="s">
+      <c r="H12" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="I12" s="21">
+      <c r="I12" s="7">
         <v>42821</v>
       </c>
-      <c r="J12" s="22" t="s">
+      <c r="J12" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="K12" s="20">
+      <c r="K12" s="6">
         <v>10</v>
       </c>
-      <c r="L12" s="23">
+      <c r="L12" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M12" s="24">
+      <c r="M12" s="10">
         <v>10</v>
       </c>
-      <c r="N12" s="20"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="25"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="11"/>
     </row>
     <row r="13" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B13" s="19"/>
-      <c r="C13" s="20" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="26" t="s">
+      <c r="E13" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="F13" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G13" s="26" t="s">
+      <c r="G13" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="H13" s="26" t="s">
+      <c r="H13" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="I13" s="30">
+      <c r="I13" s="16">
         <v>42821</v>
       </c>
-      <c r="J13" s="27" t="s">
+      <c r="J13" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="K13" s="26">
-        <v>4</v>
-      </c>
-      <c r="L13" s="23">
+      <c r="K13" s="12">
+        <v>4</v>
+      </c>
+      <c r="L13" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M13" s="28">
-        <v>4</v>
-      </c>
-      <c r="N13" s="26"/>
-      <c r="O13" s="26"/>
-      <c r="P13" s="29"/>
+      <c r="M13" s="14">
+        <v>4</v>
+      </c>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="15"/>
     </row>
     <row r="14" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B14" s="19"/>
-      <c r="C14" s="20" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="26" t="s">
+      <c r="D14" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="26" t="s">
+      <c r="E14" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="F14" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G14" s="26" t="s">
+      <c r="G14" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="H14" s="26" t="s">
+      <c r="H14" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="I14" s="21">
+      <c r="I14" s="7">
         <v>42797</v>
       </c>
-      <c r="J14" s="27" t="s">
+      <c r="J14" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="K14" s="26">
-        <v>4</v>
-      </c>
-      <c r="L14" s="23">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="M14" s="28"/>
-      <c r="N14" s="26"/>
-      <c r="O14" s="26"/>
-      <c r="P14" s="29"/>
+      <c r="K14" s="12">
+        <v>4</v>
+      </c>
+      <c r="L14" s="9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M14" s="14"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="15"/>
     </row>
     <row r="15" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B15" s="19"/>
-      <c r="C15" s="20" t="s">
+      <c r="B15" s="5"/>
+      <c r="C15" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="26" t="s">
+      <c r="D15" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="26" t="s">
+      <c r="E15" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G15" s="26" t="s">
+      <c r="G15" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="H15" s="26" t="s">
+      <c r="H15" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="I15" s="21">
+      <c r="I15" s="7">
         <v>42804</v>
       </c>
-      <c r="J15" s="27" t="s">
+      <c r="J15" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="K15" s="26">
-        <v>4</v>
-      </c>
-      <c r="L15" s="23">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="M15" s="28"/>
-      <c r="N15" s="26"/>
-      <c r="O15" s="26"/>
-      <c r="P15" s="29"/>
+      <c r="K15" s="12">
+        <v>4</v>
+      </c>
+      <c r="L15" s="9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M15" s="14"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="15"/>
     </row>
     <row r="16" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B16" s="19"/>
-      <c r="C16" s="20" t="s">
+      <c r="B16" s="5"/>
+      <c r="C16" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="26" t="s">
+      <c r="E16" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F16" s="20" t="s">
+      <c r="F16" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G16" s="26" t="s">
+      <c r="G16" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H16" s="26" t="s">
+      <c r="H16" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="I16" s="21" t="s">
+      <c r="I16" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="J16" s="27" t="s">
+      <c r="J16" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="K16" s="26">
+      <c r="K16" s="12">
         <v>16</v>
       </c>
-      <c r="L16" s="23">
+      <c r="L16" s="9">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="M16" s="28">
-        <v>4</v>
-      </c>
-      <c r="N16" s="26"/>
-      <c r="O16" s="26"/>
-      <c r="P16" s="29"/>
+      <c r="M16" s="14">
+        <v>4</v>
+      </c>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="15"/>
     </row>
     <row r="17" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B17" s="19"/>
-      <c r="C17" s="20" t="s">
+      <c r="B17" s="5"/>
+      <c r="C17" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="26" t="s">
+      <c r="D17" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="26" t="s">
+      <c r="E17" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F17" s="20" t="s">
+      <c r="F17" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G17" s="26" t="s">
+      <c r="G17" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="H17" s="26" t="s">
+      <c r="H17" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="I17" s="21" t="s">
+      <c r="I17" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="J17" s="27" t="s">
+      <c r="J17" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="K17" s="26">
+      <c r="K17" s="12">
         <v>16</v>
       </c>
-      <c r="L17" s="23">
+      <c r="L17" s="9">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="M17" s="28">
-        <v>4</v>
-      </c>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="29"/>
+      <c r="M17" s="14">
+        <v>4</v>
+      </c>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="15"/>
     </row>
     <row r="18" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B18" s="19"/>
-      <c r="C18" s="26" t="s">
+      <c r="B18" s="5"/>
+      <c r="C18" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="26" t="s">
+      <c r="D18" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="26" t="s">
+      <c r="E18" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F18" s="26" t="s">
+      <c r="F18" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G18" s="26" t="s">
+      <c r="G18" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="26" t="s">
+      <c r="H18" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="I18" s="21" t="s">
+      <c r="I18" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="J18" s="27" t="s">
+      <c r="J18" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="K18" s="26">
+      <c r="K18" s="12">
         <v>16</v>
       </c>
-      <c r="L18" s="23">
+      <c r="L18" s="9">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="M18" s="28">
-        <v>4</v>
-      </c>
-      <c r="N18" s="26"/>
-      <c r="O18" s="26"/>
-      <c r="P18" s="29"/>
+      <c r="M18" s="14">
+        <v>4</v>
+      </c>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="15"/>
     </row>
     <row r="19" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B19" s="19"/>
-      <c r="C19" s="26" t="s">
+      <c r="B19" s="5"/>
+      <c r="C19" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="26" t="s">
+      <c r="D19" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="26" t="s">
+      <c r="E19" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F19" s="26" t="s">
+      <c r="F19" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G19" s="26" t="s">
+      <c r="G19" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="26" t="s">
+      <c r="H19" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="I19" s="21" t="s">
+      <c r="I19" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="J19" s="27" t="s">
+      <c r="J19" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="K19" s="26">
+      <c r="K19" s="12">
         <v>16</v>
       </c>
-      <c r="L19" s="23">
+      <c r="L19" s="9">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="M19" s="28">
-        <v>4</v>
-      </c>
-      <c r="N19" s="26"/>
-      <c r="O19" s="26"/>
-      <c r="P19" s="29"/>
+      <c r="M19" s="14">
+        <v>4</v>
+      </c>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="15"/>
     </row>
     <row r="20" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B20" s="19"/>
-      <c r="C20" s="26" t="s">
+      <c r="B20" s="5"/>
+      <c r="C20" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="26" t="s">
+      <c r="D20" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="26" t="s">
+      <c r="E20" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="26" t="s">
+      <c r="F20" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G20" s="26" t="s">
+      <c r="G20" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H20" s="26" t="s">
+      <c r="H20" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="I20" s="21" t="s">
+      <c r="I20" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="J20" s="27" t="s">
+      <c r="J20" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="K20" s="26">
+      <c r="K20" s="12">
         <v>16</v>
       </c>
-      <c r="L20" s="23">
+      <c r="L20" s="9">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="M20" s="28">
-        <v>4</v>
-      </c>
-      <c r="N20" s="26"/>
-      <c r="O20" s="26"/>
-      <c r="P20" s="29"/>
+      <c r="M20" s="14">
+        <v>4</v>
+      </c>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="15"/>
     </row>
     <row r="21" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B21" s="19"/>
-      <c r="C21" s="26" t="s">
+      <c r="B21" s="5"/>
+      <c r="C21" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="26" t="s">
+      <c r="D21" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="26" t="s">
+      <c r="E21" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F21" s="26" t="s">
+      <c r="F21" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G21" s="26" t="s">
+      <c r="G21" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H21" s="26" t="s">
+      <c r="H21" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="I21" s="21" t="s">
+      <c r="I21" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="J21" s="27" t="s">
+      <c r="J21" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="K21" s="26">
+      <c r="K21" s="12">
         <v>16</v>
       </c>
-      <c r="L21" s="23">
+      <c r="L21" s="9">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="M21" s="28">
-        <v>4</v>
-      </c>
-      <c r="N21" s="26"/>
-      <c r="O21" s="26"/>
-      <c r="P21" s="29"/>
+      <c r="M21" s="14">
+        <v>4</v>
+      </c>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="15"/>
     </row>
     <row r="22" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B22" s="19"/>
-      <c r="C22" s="26" t="s">
+      <c r="B22" s="5"/>
+      <c r="C22" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="26" t="s">
+      <c r="D22" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="26" t="s">
+      <c r="E22" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F22" s="26" t="s">
+      <c r="F22" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G22" s="26" t="s">
+      <c r="G22" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H22" s="26" t="s">
+      <c r="H22" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="I22" s="21" t="s">
+      <c r="I22" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="J22" s="27" t="s">
+      <c r="J22" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="K22" s="26">
+      <c r="K22" s="12">
         <v>16</v>
       </c>
-      <c r="L22" s="23">
+      <c r="L22" s="9">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="M22" s="28">
-        <v>4</v>
-      </c>
-      <c r="N22" s="26"/>
-      <c r="O22" s="26"/>
-      <c r="P22" s="29"/>
+      <c r="M22" s="14">
+        <v>4</v>
+      </c>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="15"/>
     </row>
     <row r="23" spans="2:16" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="B23" s="19"/>
-      <c r="C23" s="26" t="s">
+      <c r="B23" s="5"/>
+      <c r="C23" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="26" t="s">
+      <c r="D23" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="26" t="s">
+      <c r="E23" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F23" s="26" t="s">
+      <c r="F23" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="G23" s="26" t="s">
+      <c r="G23" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="H23" s="26" t="s">
+      <c r="H23" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="I23" s="30">
+      <c r="I23" s="16">
         <v>42828</v>
       </c>
-      <c r="J23" s="27" t="s">
+      <c r="J23" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="K23" s="26">
-        <v>4</v>
-      </c>
-      <c r="L23" s="23">
+      <c r="K23" s="12">
+        <v>4</v>
+      </c>
+      <c r="L23" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M23" s="28">
-        <v>4</v>
-      </c>
-      <c r="N23" s="26"/>
-      <c r="O23" s="26"/>
-      <c r="P23" s="29"/>
+      <c r="M23" s="14">
+        <v>4</v>
+      </c>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="15"/>
     </row>
     <row r="24" spans="2:16" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="B24" s="19"/>
-      <c r="C24" s="26" t="s">
+      <c r="B24" s="5"/>
+      <c r="C24" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="26" t="s">
+      <c r="D24" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="26" t="s">
+      <c r="E24" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F24" s="26" t="s">
+      <c r="F24" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="G24" s="26" t="s">
+      <c r="G24" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="H24" s="26" t="s">
+      <c r="H24" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="I24" s="30">
+      <c r="I24" s="16">
         <v>42828</v>
       </c>
-      <c r="J24" s="27" t="s">
+      <c r="J24" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="K24" s="26">
-        <v>4</v>
-      </c>
-      <c r="L24" s="23">
+      <c r="K24" s="12">
+        <v>4</v>
+      </c>
+      <c r="L24" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M24" s="28">
-        <v>4</v>
-      </c>
-      <c r="N24" s="26"/>
-      <c r="O24" s="26"/>
-      <c r="P24" s="29"/>
+      <c r="M24" s="14">
+        <v>4</v>
+      </c>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="15"/>
     </row>
     <row r="25" spans="2:16" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="B25" s="19"/>
-      <c r="C25" s="26" t="s">
+      <c r="B25" s="5"/>
+      <c r="C25" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="26" t="s">
+      <c r="D25" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E25" s="26" t="s">
+      <c r="E25" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F25" s="26" t="s">
+      <c r="F25" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="G25" s="26" t="s">
+      <c r="G25" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="H25" s="26" t="s">
+      <c r="H25" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="I25" s="30">
+      <c r="I25" s="16">
         <v>42831</v>
       </c>
-      <c r="J25" s="27" t="s">
+      <c r="J25" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="K25" s="26">
-        <v>4</v>
-      </c>
-      <c r="L25" s="23">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="M25" s="28"/>
-      <c r="N25" s="26"/>
-      <c r="O25" s="26"/>
-      <c r="P25" s="29"/>
+      <c r="K25" s="12">
+        <v>4</v>
+      </c>
+      <c r="L25" s="9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M25" s="14"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="15"/>
     </row>
     <row r="26" spans="2:16" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="B26" s="19"/>
-      <c r="C26" s="26" t="s">
+      <c r="B26" s="5"/>
+      <c r="C26" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="26" t="s">
+      <c r="D26" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="26" t="s">
+      <c r="E26" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F26" s="26" t="s">
+      <c r="F26" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="G26" s="26" t="s">
+      <c r="G26" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="H26" s="26" t="s">
+      <c r="H26" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="I26" s="30">
+      <c r="I26" s="16">
         <v>42831</v>
       </c>
-      <c r="J26" s="27" t="s">
+      <c r="J26" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="K26" s="26">
-        <v>4</v>
-      </c>
-      <c r="L26" s="23">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="M26" s="28"/>
-      <c r="N26" s="26"/>
-      <c r="O26" s="26"/>
-      <c r="P26" s="29"/>
+      <c r="K26" s="12">
+        <v>4</v>
+      </c>
+      <c r="L26" s="9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M26" s="14"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="15"/>
     </row>
     <row r="27" spans="2:16" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="B27" s="19"/>
-      <c r="C27" s="26" t="s">
+      <c r="B27" s="5"/>
+      <c r="C27" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="26" t="s">
+      <c r="D27" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="E27" s="26" t="s">
+      <c r="E27" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F27" s="26" t="s">
+      <c r="F27" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="G27" s="26" t="s">
+      <c r="G27" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="H27" s="26" t="s">
+      <c r="H27" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="I27" s="30">
+      <c r="I27" s="16">
         <v>42831</v>
       </c>
-      <c r="J27" s="27" t="s">
+      <c r="J27" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="K27" s="26">
-        <v>4</v>
-      </c>
-      <c r="L27" s="23">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="M27" s="28"/>
-      <c r="N27" s="26"/>
-      <c r="O27" s="26"/>
-      <c r="P27" s="29"/>
+      <c r="K27" s="12">
+        <v>4</v>
+      </c>
+      <c r="L27" s="9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M27" s="14"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="15"/>
     </row>
     <row r="28" spans="2:16" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="B28" s="19"/>
-      <c r="C28" s="26" t="s">
+      <c r="B28" s="5"/>
+      <c r="C28" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D28" s="26" t="s">
+      <c r="D28" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="E28" s="26" t="s">
+      <c r="E28" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F28" s="26" t="s">
+      <c r="F28" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="G28" s="26" t="s">
+      <c r="G28" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="H28" s="26" t="s">
+      <c r="H28" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="I28" s="30">
+      <c r="I28" s="16">
         <v>42835</v>
       </c>
-      <c r="J28" s="27" t="s">
+      <c r="J28" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="K28" s="26">
-        <v>4</v>
-      </c>
-      <c r="L28" s="23">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="M28" s="28"/>
-      <c r="N28" s="26"/>
-      <c r="O28" s="26"/>
-      <c r="P28" s="29"/>
+      <c r="K28" s="12">
+        <v>4</v>
+      </c>
+      <c r="L28" s="9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M28" s="14"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="15"/>
     </row>
     <row r="29" spans="2:16" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="B29" s="19"/>
-      <c r="C29" s="26" t="s">
+      <c r="B29" s="5"/>
+      <c r="C29" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="26" t="s">
+      <c r="D29" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="E29" s="26" t="s">
+      <c r="E29" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F29" s="26" t="s">
+      <c r="F29" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="G29" s="26" t="s">
+      <c r="G29" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="H29" s="26" t="s">
+      <c r="H29" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="I29" s="30">
+      <c r="I29" s="16">
         <v>42835</v>
       </c>
-      <c r="J29" s="27" t="s">
+      <c r="J29" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="K29" s="26">
-        <v>4</v>
-      </c>
-      <c r="L29" s="23">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="M29" s="28"/>
-      <c r="N29" s="26"/>
-      <c r="O29" s="26"/>
-      <c r="P29" s="29"/>
+      <c r="K29" s="12">
+        <v>4</v>
+      </c>
+      <c r="L29" s="9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M29" s="14"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="15"/>
     </row>
     <row r="30" spans="2:16" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="B30" s="19"/>
-      <c r="C30" s="26" t="s">
+      <c r="B30" s="5"/>
+      <c r="C30" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="26" t="s">
+      <c r="D30" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="E30" s="26" t="s">
+      <c r="E30" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F30" s="26" t="s">
+      <c r="F30" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="G30" s="26" t="s">
+      <c r="G30" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="H30" s="26" t="s">
+      <c r="H30" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="I30" s="30">
+      <c r="I30" s="16">
         <v>42835</v>
       </c>
-      <c r="J30" s="27" t="s">
+      <c r="J30" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="K30" s="26">
-        <v>4</v>
-      </c>
-      <c r="L30" s="23">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="M30" s="28"/>
-      <c r="N30" s="26"/>
-      <c r="O30" s="26"/>
-      <c r="P30" s="29"/>
+      <c r="K30" s="12">
+        <v>4</v>
+      </c>
+      <c r="L30" s="9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M30" s="14"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="15"/>
     </row>
     <row r="31" spans="2:16" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="B31" s="19"/>
-      <c r="C31" s="26" t="s">
+      <c r="B31" s="5"/>
+      <c r="C31" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="26" t="s">
+      <c r="D31" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="E31" s="26" t="s">
+      <c r="E31" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F31" s="26" t="s">
+      <c r="F31" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="G31" s="26" t="s">
+      <c r="G31" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="H31" s="26" t="s">
+      <c r="H31" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="I31" s="30">
+      <c r="I31" s="16">
         <v>42835</v>
       </c>
-      <c r="J31" s="27" t="s">
+      <c r="J31" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="K31" s="26">
-        <v>4</v>
-      </c>
-      <c r="L31" s="23">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="M31" s="28"/>
-      <c r="N31" s="26"/>
-      <c r="O31" s="26"/>
-      <c r="P31" s="29"/>
+      <c r="K31" s="12">
+        <v>4</v>
+      </c>
+      <c r="L31" s="9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M31" s="14"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
+      <c r="P31" s="15"/>
     </row>
     <row r="32" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B32" s="19"/>
-      <c r="C32" s="26" t="s">
+      <c r="B32" s="5"/>
+      <c r="C32" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="26" t="s">
+      <c r="D32" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="E32" s="26" t="s">
+      <c r="E32" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F32" s="26" t="s">
+      <c r="F32" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="G32" s="26" t="s">
+      <c r="G32" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="H32" s="26" t="s">
+      <c r="H32" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="I32" s="30">
+      <c r="I32" s="16">
         <v>42828</v>
       </c>
-      <c r="J32" s="27" t="s">
+      <c r="J32" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="K32" s="26">
-        <v>2</v>
-      </c>
-      <c r="L32" s="23">
+      <c r="K32" s="12">
+        <v>2</v>
+      </c>
+      <c r="L32" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M32" s="28">
-        <v>2</v>
-      </c>
-      <c r="N32" s="26"/>
-      <c r="O32" s="26"/>
-      <c r="P32" s="29"/>
+      <c r="M32" s="14">
+        <v>2</v>
+      </c>
+      <c r="N32" s="12"/>
+      <c r="O32" s="12"/>
+      <c r="P32" s="15"/>
     </row>
     <row r="33" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B33" s="19"/>
-      <c r="C33" s="26" t="s">
+      <c r="B33" s="5"/>
+      <c r="C33" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="26" t="s">
+      <c r="D33" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="E33" s="26" t="s">
+      <c r="E33" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F33" s="26" t="s">
+      <c r="F33" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="G33" s="26" t="s">
+      <c r="G33" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="H33" s="26" t="s">
+      <c r="H33" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="I33" s="30">
+      <c r="I33" s="16">
         <v>42828</v>
       </c>
-      <c r="J33" s="27" t="s">
+      <c r="J33" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="K33" s="26">
-        <v>2</v>
-      </c>
-      <c r="L33" s="23">
+      <c r="K33" s="12">
+        <v>2</v>
+      </c>
+      <c r="L33" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M33" s="28">
-        <v>2</v>
-      </c>
-      <c r="N33" s="26"/>
-      <c r="O33" s="26"/>
-      <c r="P33" s="29"/>
+      <c r="M33" s="14">
+        <v>2</v>
+      </c>
+      <c r="N33" s="12"/>
+      <c r="O33" s="12"/>
+      <c r="P33" s="15"/>
     </row>
     <row r="34" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B34" s="19"/>
-      <c r="C34" s="26" t="s">
+      <c r="B34" s="5"/>
+      <c r="C34" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D34" s="26" t="s">
+      <c r="D34" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="E34" s="26" t="s">
+      <c r="E34" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F34" s="26" t="s">
+      <c r="F34" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="G34" s="26" t="s">
+      <c r="G34" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="H34" s="26" t="s">
+      <c r="H34" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="I34" s="30">
+      <c r="I34" s="16">
         <v>42828</v>
       </c>
-      <c r="J34" s="27" t="s">
+      <c r="J34" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="K34" s="26">
-        <v>2</v>
-      </c>
-      <c r="L34" s="23">
+      <c r="K34" s="12">
+        <v>2</v>
+      </c>
+      <c r="L34" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M34" s="28">
-        <v>2</v>
-      </c>
-      <c r="N34" s="26"/>
-      <c r="O34" s="26"/>
-      <c r="P34" s="29"/>
+      <c r="M34" s="14">
+        <v>2</v>
+      </c>
+      <c r="N34" s="12"/>
+      <c r="O34" s="12"/>
+      <c r="P34" s="15"/>
     </row>
     <row r="35" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B35" s="19"/>
-      <c r="C35" s="26" t="s">
+      <c r="B35" s="5"/>
+      <c r="C35" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D35" s="26" t="s">
+      <c r="D35" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="E35" s="26" t="s">
+      <c r="E35" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F35" s="26" t="s">
+      <c r="F35" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="G35" s="26" t="s">
+      <c r="G35" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="H35" s="26" t="s">
+      <c r="H35" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="I35" s="30">
+      <c r="I35" s="16">
         <v>42831</v>
       </c>
-      <c r="J35" s="27" t="s">
+      <c r="J35" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="K35" s="26">
-        <v>2</v>
-      </c>
-      <c r="L35" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="M35" s="28"/>
-      <c r="N35" s="26"/>
-      <c r="O35" s="26"/>
-      <c r="P35" s="29"/>
+      <c r="K35" s="12">
+        <v>2</v>
+      </c>
+      <c r="L35" s="9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M35" s="14"/>
+      <c r="N35" s="12"/>
+      <c r="O35" s="12"/>
+      <c r="P35" s="15"/>
     </row>
     <row r="36" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B36" s="19"/>
-      <c r="C36" s="26" t="s">
+      <c r="B36" s="5"/>
+      <c r="C36" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D36" s="26" t="s">
+      <c r="D36" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="E36" s="26" t="s">
+      <c r="E36" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F36" s="26" t="s">
+      <c r="F36" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="G36" s="26" t="s">
+      <c r="G36" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="H36" s="26" t="s">
+      <c r="H36" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="I36" s="30">
+      <c r="I36" s="16">
         <v>42831</v>
       </c>
-      <c r="J36" s="27" t="s">
+      <c r="J36" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="K36" s="26">
-        <v>2</v>
-      </c>
-      <c r="L36" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="M36" s="28"/>
-      <c r="N36" s="26"/>
-      <c r="O36" s="26"/>
-      <c r="P36" s="29"/>
+      <c r="K36" s="12">
+        <v>2</v>
+      </c>
+      <c r="L36" s="9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M36" s="14"/>
+      <c r="N36" s="12"/>
+      <c r="O36" s="12"/>
+      <c r="P36" s="15"/>
     </row>
     <row r="37" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B37" s="19"/>
-      <c r="C37" s="26" t="s">
+      <c r="B37" s="5"/>
+      <c r="C37" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D37" s="26" t="s">
+      <c r="D37" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="26" t="s">
+      <c r="E37" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F37" s="26" t="s">
+      <c r="F37" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="G37" s="26" t="s">
+      <c r="G37" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="H37" s="26" t="s">
+      <c r="H37" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="I37" s="30">
+      <c r="I37" s="16">
         <v>42831</v>
       </c>
-      <c r="J37" s="27" t="s">
+      <c r="J37" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="K37" s="26">
-        <v>2</v>
-      </c>
-      <c r="L37" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="M37" s="28"/>
-      <c r="N37" s="26"/>
-      <c r="O37" s="26"/>
-      <c r="P37" s="29"/>
+      <c r="K37" s="12">
+        <v>2</v>
+      </c>
+      <c r="L37" s="9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M37" s="14"/>
+      <c r="N37" s="12"/>
+      <c r="O37" s="12"/>
+      <c r="P37" s="15"/>
     </row>
     <row r="38" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B38" s="19"/>
-      <c r="C38" s="26" t="s">
+      <c r="B38" s="5"/>
+      <c r="C38" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D38" s="26" t="s">
+      <c r="D38" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="E38" s="26" t="s">
+      <c r="E38" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F38" s="26" t="s">
+      <c r="F38" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="G38" s="26" t="s">
+      <c r="G38" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="H38" s="26" t="s">
+      <c r="H38" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="I38" s="30">
+      <c r="I38" s="16">
         <v>42835</v>
       </c>
-      <c r="J38" s="27" t="s">
+      <c r="J38" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="K38" s="26">
-        <v>2</v>
-      </c>
-      <c r="L38" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="M38" s="28"/>
-      <c r="N38" s="26"/>
-      <c r="O38" s="26"/>
-      <c r="P38" s="29"/>
+      <c r="K38" s="12">
+        <v>2</v>
+      </c>
+      <c r="L38" s="9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M38" s="14"/>
+      <c r="N38" s="12"/>
+      <c r="O38" s="12"/>
+      <c r="P38" s="15"/>
     </row>
     <row r="39" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B39" s="19"/>
-      <c r="C39" s="26" t="s">
+      <c r="B39" s="5"/>
+      <c r="C39" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D39" s="26" t="s">
+      <c r="D39" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="E39" s="26" t="s">
+      <c r="E39" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F39" s="26" t="s">
+      <c r="F39" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="G39" s="26" t="s">
+      <c r="G39" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="H39" s="26" t="s">
+      <c r="H39" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="I39" s="30">
+      <c r="I39" s="16">
         <v>42835</v>
       </c>
-      <c r="J39" s="27" t="s">
+      <c r="J39" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="K39" s="26">
-        <v>2</v>
-      </c>
-      <c r="L39" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="M39" s="28"/>
-      <c r="N39" s="26"/>
-      <c r="O39" s="26"/>
-      <c r="P39" s="29"/>
+      <c r="K39" s="12">
+        <v>2</v>
+      </c>
+      <c r="L39" s="9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M39" s="14"/>
+      <c r="N39" s="12"/>
+      <c r="O39" s="12"/>
+      <c r="P39" s="15"/>
     </row>
     <row r="40" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B40" s="19"/>
-      <c r="C40" s="26" t="s">
+      <c r="B40" s="5"/>
+      <c r="C40" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D40" s="26" t="s">
+      <c r="D40" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="26" t="s">
+      <c r="E40" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F40" s="26" t="s">
+      <c r="F40" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="G40" s="26" t="s">
+      <c r="G40" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="H40" s="26" t="s">
+      <c r="H40" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="I40" s="30">
+      <c r="I40" s="16">
         <v>42835</v>
       </c>
-      <c r="J40" s="27" t="s">
+      <c r="J40" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="K40" s="26">
-        <v>2</v>
-      </c>
-      <c r="L40" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="M40" s="28"/>
-      <c r="N40" s="26"/>
-      <c r="O40" s="26"/>
-      <c r="P40" s="29"/>
+      <c r="K40" s="12">
+        <v>2</v>
+      </c>
+      <c r="L40" s="9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M40" s="14"/>
+      <c r="N40" s="12"/>
+      <c r="O40" s="12"/>
+      <c r="P40" s="15"/>
     </row>
     <row r="41" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B41" s="19"/>
-      <c r="C41" s="26" t="s">
+      <c r="B41" s="5"/>
+      <c r="C41" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="D41" s="26" t="s">
+      <c r="D41" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="E41" s="26" t="s">
+      <c r="E41" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F41" s="26" t="s">
+      <c r="F41" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="G41" s="26" t="s">
+      <c r="G41" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="H41" s="26" t="s">
+      <c r="H41" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="I41" s="30" t="s">
+      <c r="I41" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="J41" s="27" t="s">
+      <c r="J41" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="K41" s="26">
+      <c r="K41" s="12">
         <v>16</v>
       </c>
-      <c r="L41" s="23">
+      <c r="L41" s="9">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="M41" s="28">
-        <v>4</v>
-      </c>
-      <c r="N41" s="26"/>
-      <c r="O41" s="26"/>
-      <c r="P41" s="29"/>
+      <c r="M41" s="14">
+        <v>4</v>
+      </c>
+      <c r="N41" s="12"/>
+      <c r="O41" s="12"/>
+      <c r="P41" s="15"/>
     </row>
     <row r="42" spans="2:16" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="B42" s="19"/>
-      <c r="C42" s="26" t="s">
+      <c r="B42" s="5"/>
+      <c r="C42" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="D42" s="26" t="s">
+      <c r="D42" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="E42" s="26" t="s">
+      <c r="E42" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F42" s="26" t="s">
+      <c r="F42" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="G42" s="26" t="s">
+      <c r="G42" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="H42" s="26" t="s">
+      <c r="H42" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="I42" s="30">
-        <v>42838</v>
-      </c>
-      <c r="J42" s="27" t="s">
+      <c r="I42" s="16">
+        <v>42843</v>
+      </c>
+      <c r="J42" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="K42" s="26">
-        <v>2</v>
-      </c>
-      <c r="L42" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="M42" s="28"/>
-      <c r="N42" s="26"/>
-      <c r="O42" s="26"/>
-      <c r="P42" s="29"/>
+      <c r="K42" s="12">
+        <v>2</v>
+      </c>
+      <c r="L42" s="9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M42" s="14"/>
+      <c r="N42" s="12"/>
+      <c r="O42" s="12"/>
+      <c r="P42" s="15"/>
     </row>
     <row r="43" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B43" s="19"/>
-      <c r="C43" s="26" t="s">
+      <c r="B43" s="5"/>
+      <c r="C43" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="D43" s="26" t="s">
+      <c r="D43" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="E43" s="26" t="s">
+      <c r="E43" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F43" s="26" t="s">
+      <c r="F43" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="G43" s="26" t="s">
+      <c r="G43" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="H43" s="26" t="s">
+      <c r="H43" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="I43" s="30">
+      <c r="I43" s="16">
         <v>42815</v>
       </c>
-      <c r="J43" s="27" t="s">
+      <c r="J43" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="K43" s="26">
-        <v>2</v>
-      </c>
-      <c r="L43" s="23">
+      <c r="K43" s="12">
+        <v>2</v>
+      </c>
+      <c r="L43" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M43" s="28">
-        <v>2</v>
-      </c>
-      <c r="N43" s="26"/>
-      <c r="O43" s="26"/>
-      <c r="P43" s="29"/>
+      <c r="M43" s="14">
+        <v>2</v>
+      </c>
+      <c r="N43" s="12"/>
+      <c r="O43" s="12"/>
+      <c r="P43" s="15"/>
     </row>
     <row r="44" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B44" s="19"/>
-      <c r="C44" s="26" t="s">
+      <c r="B44" s="5"/>
+      <c r="C44" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="D44" s="26" t="s">
+      <c r="D44" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="E44" s="26" t="s">
+      <c r="E44" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F44" s="26" t="s">
+      <c r="F44" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="G44" s="26" t="s">
+      <c r="G44" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="H44" s="26" t="s">
+      <c r="H44" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="I44" s="30">
+      <c r="I44" s="16">
         <v>42797</v>
       </c>
-      <c r="J44" s="27" t="s">
+      <c r="J44" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="K44" s="26">
-        <v>4</v>
-      </c>
-      <c r="L44" s="23">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="M44" s="28"/>
-      <c r="N44" s="26"/>
-      <c r="O44" s="26"/>
-      <c r="P44" s="29"/>
+      <c r="K44" s="12">
+        <v>4</v>
+      </c>
+      <c r="L44" s="9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M44" s="14"/>
+      <c r="N44" s="12"/>
+      <c r="O44" s="12"/>
+      <c r="P44" s="15"/>
     </row>
     <row r="45" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B45" s="19"/>
-      <c r="C45" s="26" t="s">
+      <c r="B45" s="5"/>
+      <c r="C45" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="D45" s="26" t="s">
+      <c r="D45" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="E45" s="26" t="s">
+      <c r="E45" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="F45" s="26" t="s">
+      <c r="F45" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="G45" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="H45" s="26" t="s">
+      <c r="G45" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H45" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="I45" s="30" t="s">
+      <c r="I45" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="J45" s="27" t="s">
+      <c r="J45" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="K45" s="26">
-        <v>4</v>
-      </c>
-      <c r="L45" s="23">
+      <c r="K45" s="12">
+        <v>4</v>
+      </c>
+      <c r="L45" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="M45" s="28">
+      <c r="M45" s="14">
         <v>1</v>
       </c>
-      <c r="N45" s="26"/>
-      <c r="O45" s="26"/>
-      <c r="P45" s="29"/>
+      <c r="N45" s="12"/>
+      <c r="O45" s="12"/>
+      <c r="P45" s="15"/>
     </row>
     <row r="48" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C48" s="31"/>
-      <c r="D48" s="32"/>
-      <c r="J48" s="31"/>
-      <c r="L48" s="31"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="18"/>
+      <c r="J48" s="17"/>
+      <c r="L48" s="17"/>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D49" s="32"/>
+      <c r="D49" s="18"/>
     </row>
     <row r="50" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D50" s="32"/>
+      <c r="D50" s="18"/>
     </row>
     <row r="51" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D51" s="32"/>
+      <c r="D51" s="18"/>
     </row>
     <row r="52" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D52" s="32"/>
+      <c r="D52" s="18"/>
     </row>
     <row r="53" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D53" s="32"/>
+      <c r="D53" s="18"/>
     </row>
     <row r="54" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D54" s="32"/>
+      <c r="D54" s="18"/>
     </row>
     <row r="55" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D55" s="32"/>
+      <c r="D55" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -2702,12 +2705,12 @@
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:P5"/>
+    <mergeCell ref="G5:G6"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>